<commit_message>
Changed HDR Breast Colours
</commit_message>
<xml_diff>
--- a/External Beam Templates/Structure Templates/Template Spreadsheets/HDR Templates.xlsx
+++ b/External Beam Templates/Structure Templates/Template Spreadsheets/HDR Templates.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="555" windowWidth="27030" windowHeight="9885"/>
+    <workbookView xWindow="9585" yWindow="-15" windowWidth="9600" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="HDR BREAST" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="104">
   <si>
     <t>HDR BREAST</t>
   </si>
@@ -316,6 +316,21 @@
   </si>
   <si>
     <t>TemplateFileName</t>
+  </si>
+  <si>
+    <t>Transluce - Red</t>
+  </si>
+  <si>
+    <t>Translucent-Purp</t>
+  </si>
+  <si>
+    <t>Transluce - Pink</t>
+  </si>
+  <si>
+    <t>Transluce - Lila</t>
+  </si>
+  <si>
+    <t>Transluce - Blue</t>
   </si>
 </sst>
 </file>
@@ -618,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -737,6 +752,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1267,39 +1285,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1319,22 +1310,6 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1354,22 +1329,6 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1388,20 +1347,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1431,35 +1376,6 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1577,14 +1493,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table5337911" displayName="Table5337911" ref="D2:H17" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table5337911" displayName="Table5337911" ref="D2:I17" totalsRowShown="0" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <sortState ref="D3:H15">
     <sortCondition ref="E3:E15"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Structure" dataDxfId="30"/>
-    <tableColumn id="2" name="ID" dataDxfId="29"/>
-    <tableColumn id="3" name="Name" dataDxfId="28"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Structure" dataDxfId="31"/>
+    <tableColumn id="2" name="ID" dataDxfId="30"/>
+    <tableColumn id="3" name="Name" dataDxfId="29"/>
+    <tableColumn id="6" name="ColorAndStyle" dataDxfId="28"/>
     <tableColumn id="4" name="VolumeCode" dataDxfId="27"/>
     <tableColumn id="5" name="VolumeCodeTable" dataDxfId="26"/>
   </tableColumns>
@@ -1934,10 +1851,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,59 +1867,61 @@
     <col min="6" max="6" width="39.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="20.7109375" style="47" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:22" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="51"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="J1" s="48" t="s">
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="48"/>
+      <c r="K1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="48" t="s">
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="51"/>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="52"/>
+      <c r="Q1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="R1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="48" t="s">
+      <c r="S1" s="52"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="49"/>
+      <c r="V1" s="50"/>
     </row>
-    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -2010,59 +1929,62 @@
         <v>8</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="Q2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="T2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="U2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="V2" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>81</v>
       </c>
@@ -2070,67 +1992,67 @@
         <v>0</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="15"/>
-      <c r="J3" s="19" t="str">
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="K3" s="19" t="str">
         <f>VLOOKUP(D3,[1]!Dictionary[#All],3,FALSE)</f>
         <v>Body</v>
       </c>
-      <c r="K3" s="20" t="str">
+      <c r="L3" s="20" t="str">
         <f>VLOOKUP(D3,[1]!Dictionary[#All],4,FALSE)</f>
         <v>BODY</v>
       </c>
-      <c r="L3" s="20" t="str">
+      <c r="M3" s="20" t="str">
         <f>VLOOKUP(D3,[1]!Dictionary[#All],5,FALSE)</f>
         <v>99VMS_STRUCTCODE</v>
       </c>
-      <c r="M3" s="21" t="str">
+      <c r="N3" s="21" t="str">
         <f>VLOOKUP(D3,[1]!Dictionary[#All],6,FALSE)</f>
         <v>1.0</v>
       </c>
-      <c r="N3" s="22" t="str">
+      <c r="O3" s="22" t="str">
         <f>VLOOKUP(D3,[1]!VolumeType[#All],2,FALSE)</f>
         <v>Special</v>
       </c>
-      <c r="O3" s="23" t="str">
+      <c r="P3" s="23" t="str">
         <f>VLOOKUP(D3,[1]!VolumeType[#All],3,FALSE)</f>
         <v>BODY</v>
       </c>
-      <c r="P3" s="24" t="str">
-        <f>VLOOKUP(D3,[1]!Colors[#All],3,FALSE)</f>
+      <c r="Q3" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D3,[1]!Colors[#All],3,FALSE))</f>
         <v>z Body</v>
       </c>
-      <c r="Q3" s="25" t="str">
+      <c r="R3" s="25" t="str">
         <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R3" s="26" t="str">
+      <c r="S3" s="26" t="str">
         <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S3" s="27" t="str">
+      <c r="T3" s="27" t="str">
         <f>IFERROR(VLOOKUP(D3,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T3" s="25">
+      <c r="U3" s="25">
         <f>IFERROR(VLOOKUP(D3,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v>-350</v>
       </c>
-      <c r="U3" s="27">
+      <c r="V3" s="27">
         <f>IFERROR(VLOOKUP(D3,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v>-50</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>83</v>
       </c>
@@ -2138,67 +2060,69 @@
         <v>9</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="15"/>
-      <c r="J4" s="19" t="str">
+      <c r="G4" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="47"/>
+      <c r="K4" s="19" t="str">
         <f>VLOOKUP(D4,[1]!Dictionary[#All],3,FALSE)</f>
         <v>CTV Intermediate Risk</v>
       </c>
-      <c r="K4" s="20" t="str">
+      <c r="L4" s="20" t="str">
         <f>VLOOKUP(D4,[1]!Dictionary[#All],4,FALSE)</f>
         <v>CTV_Intermediate</v>
       </c>
-      <c r="L4" s="20" t="str">
+      <c r="M4" s="20" t="str">
         <f>VLOOKUP(D4,[1]!Dictionary[#All],5,FALSE)</f>
         <v>99VMS_STRUCTCODE</v>
       </c>
-      <c r="M4" s="21" t="str">
+      <c r="N4" s="21" t="str">
         <f>VLOOKUP(D4,[1]!Dictionary[#All],6,FALSE)</f>
         <v>1.0</v>
       </c>
-      <c r="N4" s="22" t="str">
+      <c r="O4" s="22" t="str">
         <f>VLOOKUP(D4,[1]!VolumeType[#All],2,FALSE)</f>
         <v>CTV</v>
       </c>
-      <c r="O4" s="23" t="str">
+      <c r="P4" s="23" t="str">
         <f>VLOOKUP(D4,[1]!VolumeType[#All],3,FALSE)</f>
         <v>CTV</v>
       </c>
-      <c r="P4" s="24" t="str">
-        <f>VLOOKUP(D4,[1]!Colors[#All],3,FALSE)</f>
-        <v>z CTV int</v>
-      </c>
-      <c r="Q4" s="25" t="str">
+      <c r="Q4" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D4,[1]!Colors[#All],3,FALSE))</f>
+        <v>Transluce - Red</v>
+      </c>
+      <c r="R4" s="25" t="str">
         <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R4" s="26" t="str">
+      <c r="S4" s="26" t="str">
         <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S4" s="27" t="str">
+      <c r="T4" s="27" t="str">
         <f>IFERROR(VLOOKUP(D4,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T4" s="25" t="str">
+      <c r="U4" s="25" t="str">
         <f>IFERROR(VLOOKUP(D4,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U4" s="27" t="str">
+      <c r="V4" s="27" t="str">
         <f>IFERROR(VLOOKUP(D4,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
         <v>31</v>
       </c>
@@ -2206,852 +2130,860 @@
         <v>32</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="15"/>
-      <c r="J5" s="19" t="str">
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="K5" s="19" t="str">
         <f>VLOOKUP(D5,[1]!Dictionary[#All],3,FALSE)</f>
         <v>Intercostal muscle</v>
       </c>
-      <c r="K5" s="20">
+      <c r="L5" s="20">
         <f>VLOOKUP(D5,[1]!Dictionary[#All],4,FALSE)</f>
         <v>13354</v>
       </c>
-      <c r="L5" s="20" t="str">
+      <c r="M5" s="20" t="str">
         <f>VLOOKUP(D5,[1]!Dictionary[#All],5,FALSE)</f>
         <v>FMA</v>
       </c>
-      <c r="M5" s="21" t="str">
+      <c r="N5" s="21" t="str">
         <f>VLOOKUP(D5,[1]!Dictionary[#All],6,FALSE)</f>
         <v>3.2</v>
       </c>
-      <c r="N5" s="22" t="str">
+      <c r="O5" s="22" t="str">
         <f>VLOOKUP(D5,[1]!VolumeType[#All],2,FALSE)</f>
         <v>Organ</v>
       </c>
-      <c r="O5" s="23" t="str">
+      <c r="P5" s="23" t="str">
         <f>VLOOKUP(D5,[1]!VolumeType[#All],3,FALSE)</f>
         <v>Organ</v>
       </c>
-      <c r="P5" s="24" t="str">
-        <f>VLOOKUP(D5,[1]!Colors[#All],3,FALSE)</f>
+      <c r="Q5" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D5,[1]!Colors[#All],3,FALSE))</f>
         <v>zIntercostmuscle</v>
       </c>
-      <c r="Q5" s="25" t="str">
+      <c r="R5" s="25" t="str">
         <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R5" s="26" t="str">
+      <c r="S5" s="26" t="str">
         <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S5" s="27" t="str">
+      <c r="T5" s="27" t="str">
         <f>IFERROR(VLOOKUP(D5,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T5" s="25" t="str">
+      <c r="U5" s="25" t="str">
         <f>IFERROR(VLOOKUP(D5,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U5" s="27" t="str">
+      <c r="V5" s="27" t="str">
         <f>IFERROR(VLOOKUP(D5,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="F6"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="15"/>
-      <c r="J6" s="19" t="str">
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="K6" s="19" t="str">
         <f>VLOOKUP(D6,[1]!Dictionary[#All],3,FALSE)</f>
         <v>CTV High Risk</v>
       </c>
-      <c r="K6" s="20" t="str">
+      <c r="L6" s="20" t="str">
         <f>VLOOKUP(D6,[1]!Dictionary[#All],4,FALSE)</f>
         <v>CTV_High</v>
       </c>
-      <c r="L6" s="20" t="str">
+      <c r="M6" s="20" t="str">
         <f>VLOOKUP(D6,[1]!Dictionary[#All],5,FALSE)</f>
         <v>99VMS_STRUCTCODE</v>
       </c>
-      <c r="M6" s="21" t="str">
+      <c r="N6" s="21" t="str">
         <f>VLOOKUP(D6,[1]!Dictionary[#All],6,FALSE)</f>
         <v>1.0</v>
       </c>
-      <c r="N6" s="22" t="str">
+      <c r="O6" s="22" t="str">
         <f>VLOOKUP(D6,[1]!VolumeType[#All],2,FALSE)</f>
         <v>CTV</v>
       </c>
-      <c r="O6" s="23" t="str">
+      <c r="P6" s="23" t="str">
         <f>VLOOKUP(D6,[1]!VolumeType[#All],3,FALSE)</f>
         <v>CTV</v>
       </c>
-      <c r="P6" s="24" t="str">
-        <f>VLOOKUP(D6,[1]!Colors[#All],3,FALSE)</f>
+      <c r="Q6" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D6,[1]!Colors[#All],3,FALSE))</f>
         <v>z CTV</v>
       </c>
-      <c r="Q6" s="25" t="str">
+      <c r="R6" s="25" t="str">
         <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R6" s="26" t="str">
+      <c r="S6" s="26" t="str">
         <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S6" s="27" t="str">
+      <c r="T6" s="27" t="str">
         <f>IFERROR(VLOOKUP(D6,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T6" s="25" t="str">
+      <c r="U6" s="25" t="str">
         <f>IFERROR(VLOOKUP(D6,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U6" s="27" t="str">
+      <c r="V6" s="27" t="str">
         <f>IFERROR(VLOOKUP(D6,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="15"/>
-      <c r="J7" s="19" t="str">
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="K7" s="19" t="str">
         <f>VLOOKUP(D7,[1]!Dictionary[#All],3,FALSE)</f>
         <v>Treated Volume</v>
       </c>
-      <c r="K7" s="20" t="str">
+      <c r="L7" s="20" t="str">
         <f>VLOOKUP(D7,[1]!Dictionary[#All],4,FALSE)</f>
         <v>Treated Volume</v>
       </c>
-      <c r="L7" s="20" t="str">
+      <c r="M7" s="20" t="str">
         <f>VLOOKUP(D7,[1]!Dictionary[#All],5,FALSE)</f>
         <v>99VMS_STRUCTCODE</v>
       </c>
-      <c r="M7" s="21" t="str">
+      <c r="N7" s="21" t="str">
         <f>VLOOKUP(D7,[1]!Dictionary[#All],6,FALSE)</f>
         <v>1.0</v>
       </c>
-      <c r="N7" s="22" t="str">
+      <c r="O7" s="22" t="str">
         <f>VLOOKUP(D7,[1]!VolumeType[#All],2,FALSE)</f>
         <v>Special</v>
       </c>
-      <c r="O7" s="23" t="str">
+      <c r="P7" s="23" t="str">
         <f>VLOOKUP(D7,[1]!VolumeType[#All],3,FALSE)</f>
         <v>PTV</v>
       </c>
-      <c r="P7" s="24" t="str">
-        <f>VLOOKUP(D7,[1]!Colors[#All],3,FALSE)</f>
+      <c r="Q7" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D7,[1]!Colors[#All],3,FALSE))</f>
         <v>z DPV</v>
       </c>
-      <c r="Q7" s="25" t="str">
+      <c r="R7" s="25" t="str">
         <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R7" s="26" t="str">
+      <c r="S7" s="26" t="str">
         <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S7" s="27" t="str">
+      <c r="T7" s="27" t="str">
         <f>IFERROR(VLOOKUP(D7,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T7" s="25" t="str">
+      <c r="U7" s="25" t="str">
         <f>IFERROR(VLOOKUP(D7,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U7" s="27" t="str">
+      <c r="V7" s="27" t="str">
         <f>IFERROR(VLOOKUP(D7,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
-      <c r="J8" s="19" t="str">
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="K8" s="19" t="str">
         <f>VLOOKUP(D8,[1]!Dictionary[#All],3,FALSE)</f>
         <v>Heart</v>
       </c>
-      <c r="K8" s="20">
+      <c r="L8" s="20">
         <f>VLOOKUP(D8,[1]!Dictionary[#All],4,FALSE)</f>
         <v>7088</v>
       </c>
-      <c r="L8" s="20" t="str">
+      <c r="M8" s="20" t="str">
         <f>VLOOKUP(D8,[1]!Dictionary[#All],5,FALSE)</f>
         <v>FMA</v>
       </c>
-      <c r="M8" s="21" t="str">
+      <c r="N8" s="21" t="str">
         <f>VLOOKUP(D8,[1]!Dictionary[#All],6,FALSE)</f>
         <v>3.2</v>
       </c>
-      <c r="N8" s="22" t="str">
+      <c r="O8" s="22" t="str">
         <f>VLOOKUP(D8,[1]!VolumeType[#All],2,FALSE)</f>
         <v>Organ</v>
       </c>
-      <c r="O8" s="23" t="str">
+      <c r="P8" s="23" t="str">
         <f>VLOOKUP(D8,[1]!VolumeType[#All],3,FALSE)</f>
         <v>Organ</v>
       </c>
-      <c r="P8" s="24" t="str">
-        <f>VLOOKUP(D8,[1]!Colors[#All],3,FALSE)</f>
+      <c r="Q8" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D8,[1]!Colors[#All],3,FALSE))</f>
         <v>z Heart</v>
       </c>
-      <c r="Q8" s="25" t="str">
+      <c r="R8" s="25" t="str">
         <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R8" s="26" t="str">
+      <c r="S8" s="26" t="str">
         <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S8" s="27" t="str">
+      <c r="T8" s="27" t="str">
         <f>IFERROR(VLOOKUP(D8,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T8" s="25" t="str">
+      <c r="U8" s="25" t="str">
         <f>IFERROR(VLOOKUP(D8,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U8" s="27" t="str">
+      <c r="V8" s="27" t="str">
         <f>IFERROR(VLOOKUP(D8,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>82</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
-      <c r="J9" s="19" t="str">
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="K9" s="19" t="str">
         <f>VLOOKUP(D9,[1]!Dictionary[#All],3,FALSE)</f>
         <v>PTV Primary</v>
       </c>
-      <c r="K9" s="20" t="str">
+      <c r="L9" s="20" t="str">
         <f>VLOOKUP(D9,[1]!Dictionary[#All],4,FALSE)</f>
         <v>PTVp</v>
       </c>
-      <c r="L9" s="20" t="str">
+      <c r="M9" s="20" t="str">
         <f>VLOOKUP(D9,[1]!Dictionary[#All],5,FALSE)</f>
         <v>99VMS_STRUCTCODE</v>
       </c>
-      <c r="M9" s="21" t="str">
+      <c r="N9" s="21" t="str">
         <f>VLOOKUP(D9,[1]!Dictionary[#All],6,FALSE)</f>
         <v>1.0</v>
       </c>
-      <c r="N9" s="22" t="str">
+      <c r="O9" s="22" t="str">
         <f>VLOOKUP(D9,[1]!VolumeType[#All],2,FALSE)</f>
         <v>PTV</v>
       </c>
-      <c r="O9" s="23" t="str">
+      <c r="P9" s="23" t="str">
         <f>VLOOKUP(D9,[1]!VolumeType[#All],3,FALSE)</f>
         <v>PTV</v>
       </c>
-      <c r="P9" s="24" t="str">
-        <f>VLOOKUP(D9,[1]!Colors[#All],3,FALSE)</f>
+      <c r="Q9" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D9,[1]!Colors[#All],3,FALSE))</f>
         <v>z PTV</v>
       </c>
-      <c r="Q9" s="25" t="str">
+      <c r="R9" s="25" t="str">
         <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R9" s="26" t="str">
+      <c r="S9" s="26" t="str">
         <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S9" s="27" t="str">
+      <c r="T9" s="27" t="str">
         <f>IFERROR(VLOOKUP(D9,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T9" s="25" t="str">
+      <c r="U9" s="25" t="str">
         <f>IFERROR(VLOOKUP(D9,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U9" s="27" t="str">
+      <c r="V9" s="27" t="str">
         <f>IFERROR(VLOOKUP(D9,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
         <v>74</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="35"/>
-      <c r="J10" s="19" t="str">
+      <c r="G10" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="47"/>
+      <c r="K10" s="19" t="str">
         <f>VLOOKUP(D10,[1]!Dictionary[#All],3,FALSE)</f>
         <v>PTV Primary</v>
       </c>
-      <c r="K10" s="20" t="str">
+      <c r="L10" s="20" t="str">
         <f>VLOOKUP(D10,[1]!Dictionary[#All],4,FALSE)</f>
         <v>PTVp</v>
       </c>
-      <c r="L10" s="20" t="str">
+      <c r="M10" s="20" t="str">
         <f>VLOOKUP(D10,[1]!Dictionary[#All],5,FALSE)</f>
         <v>99VMS_STRUCTCODE</v>
       </c>
-      <c r="M10" s="21" t="str">
+      <c r="N10" s="21" t="str">
         <f>VLOOKUP(D10,[1]!Dictionary[#All],6,FALSE)</f>
         <v>1.0</v>
       </c>
-      <c r="N10" s="22" t="str">
+      <c r="O10" s="22" t="str">
         <f>VLOOKUP(D10,[1]!VolumeType[#All],2,FALSE)</f>
         <v>PTV</v>
       </c>
-      <c r="O10" s="23" t="str">
+      <c r="P10" s="23" t="str">
         <f>VLOOKUP(D10,[1]!VolumeType[#All],3,FALSE)</f>
         <v>PTV</v>
       </c>
-      <c r="P10" s="24" t="str">
-        <f>VLOOKUP(D10,[1]!Colors[#All],3,FALSE)</f>
-        <v>z PTV eval</v>
-      </c>
-      <c r="Q10" s="25">
+      <c r="Q10" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D10,[1]!Colors[#All],3,FALSE))</f>
+        <v>Transluce - Blue</v>
+      </c>
+      <c r="R10" s="25">
         <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v>-16777216</v>
       </c>
-      <c r="R10" s="26">
+      <c r="S10" s="26">
         <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v>0</v>
       </c>
-      <c r="S10" s="27">
+      <c r="T10" s="27">
         <f>IFERROR(VLOOKUP(D10,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v>5</v>
       </c>
-      <c r="T10" s="25" t="str">
+      <c r="U10" s="25" t="str">
         <f>IFERROR(VLOOKUP(D10,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U10" s="27" t="str">
+      <c r="V10" s="27" t="str">
         <f>IFERROR(VLOOKUP(D10,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
         <v>98</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-      <c r="J11" s="19" t="str">
+      <c r="G11" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="47"/>
+      <c r="K11" s="19" t="str">
         <f>VLOOKUP(D11,[1]!Dictionary[#All],3,FALSE)</f>
         <v>PTV Intermediate Risk</v>
       </c>
-      <c r="K11" s="20" t="str">
+      <c r="L11" s="20" t="str">
         <f>VLOOKUP(D11,[1]!Dictionary[#All],4,FALSE)</f>
         <v>PTV_Intermediate</v>
       </c>
-      <c r="L11" s="20" t="str">
+      <c r="M11" s="20" t="str">
         <f>VLOOKUP(D11,[1]!Dictionary[#All],5,FALSE)</f>
         <v>99VMS_STRUCTCODE</v>
       </c>
-      <c r="M11" s="21" t="str">
+      <c r="N11" s="21" t="str">
         <f>VLOOKUP(D11,[1]!Dictionary[#All],6,FALSE)</f>
         <v>1.0</v>
       </c>
-      <c r="N11" s="22" t="str">
+      <c r="O11" s="22" t="str">
         <f>VLOOKUP(D11,[1]!VolumeType[#All],2,FALSE)</f>
         <v>PTV</v>
       </c>
-      <c r="O11" s="23" t="str">
+      <c r="P11" s="23" t="str">
         <f>VLOOKUP(D11,[1]!VolumeType[#All],3,FALSE)</f>
         <v>PTV</v>
       </c>
-      <c r="P11" s="24" t="str">
-        <f>VLOOKUP(D11,[1]!Colors[#All],3,FALSE)</f>
-        <v>z PTV int</v>
-      </c>
-      <c r="Q11" s="25" t="str">
+      <c r="Q11" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D11,[1]!Colors[#All],3,FALSE))</f>
+        <v>Translucent-Purp</v>
+      </c>
+      <c r="R11" s="25" t="str">
         <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R11" s="26" t="str">
+      <c r="S11" s="26" t="str">
         <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S11" s="27" t="str">
+      <c r="T11" s="27" t="str">
         <f>IFERROR(VLOOKUP(D11,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T11" s="25" t="str">
+      <c r="U11" s="25" t="str">
         <f>IFERROR(VLOOKUP(D11,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U11" s="27" t="str">
+      <c r="V11" s="27" t="str">
         <f>IFERROR(VLOOKUP(D11,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
         <v>76</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="34"/>
-      <c r="H12" s="35"/>
-      <c r="J12" s="19" t="str">
+      <c r="G12" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="47"/>
+      <c r="K12" s="19" t="str">
         <f>VLOOKUP(D12,[1]!Dictionary[#All],3,FALSE)</f>
         <v>PTV Intermediate Risk</v>
       </c>
-      <c r="K12" s="20" t="str">
+      <c r="L12" s="20" t="str">
         <f>VLOOKUP(D12,[1]!Dictionary[#All],4,FALSE)</f>
         <v>PTV_Intermediate</v>
       </c>
-      <c r="L12" s="20" t="str">
+      <c r="M12" s="20" t="str">
         <f>VLOOKUP(D12,[1]!Dictionary[#All],5,FALSE)</f>
         <v>99VMS_STRUCTCODE</v>
       </c>
-      <c r="M12" s="21" t="str">
+      <c r="N12" s="21" t="str">
         <f>VLOOKUP(D12,[1]!Dictionary[#All],6,FALSE)</f>
         <v>1.0</v>
       </c>
-      <c r="N12" s="22" t="str">
+      <c r="O12" s="22" t="str">
         <f>VLOOKUP(D12,[1]!VolumeType[#All],2,FALSE)</f>
         <v>PTV</v>
       </c>
-      <c r="O12" s="23" t="str">
+      <c r="P12" s="23" t="str">
         <f>VLOOKUP(D12,[1]!VolumeType[#All],3,FALSE)</f>
         <v>PTV</v>
       </c>
-      <c r="P12" s="24" t="str">
-        <f>VLOOKUP(D12,[1]!Colors[#All],3,FALSE)</f>
-        <v>z PTV int eval</v>
-      </c>
-      <c r="Q12" s="25">
+      <c r="Q12" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D12,[1]!Colors[#All],3,FALSE))</f>
+        <v>Transluce - Pink</v>
+      </c>
+      <c r="R12" s="25">
         <f>IFERROR(VLOOKUP(D12,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v>-16777216</v>
       </c>
-      <c r="R12" s="26">
+      <c r="S12" s="26">
         <f>IFERROR(VLOOKUP(D12,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v>0</v>
       </c>
-      <c r="S12" s="27">
+      <c r="T12" s="27">
         <f>IFERROR(VLOOKUP(D12,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v>5</v>
       </c>
-      <c r="T12" s="25" t="str">
+      <c r="U12" s="25" t="str">
         <f>IFERROR(VLOOKUP(D12,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U12" s="27" t="str">
+      <c r="V12" s="27" t="str">
         <f>IFERROR(VLOOKUP(D12,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="29" t="s">
+      <c r="E13" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="35"/>
-      <c r="J13" s="19" t="str">
+      <c r="G13" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="47"/>
+      <c r="K13" s="19" t="str">
         <f>VLOOKUP(D13,[1]!Dictionary[#All],3,FALSE)</f>
         <v>Wire</v>
       </c>
-      <c r="K13" s="20">
+      <c r="L13" s="20">
         <f>VLOOKUP(D13,[1]!Dictionary[#All],4,FALSE)</f>
         <v>5453</v>
       </c>
-      <c r="L13" s="20" t="str">
+      <c r="M13" s="20" t="str">
         <f>VLOOKUP(D13,[1]!Dictionary[#All],5,FALSE)</f>
         <v>RADLEX</v>
       </c>
-      <c r="M13" s="21">
+      <c r="N13" s="21">
         <f>VLOOKUP(D13,[1]!Dictionary[#All],6,FALSE)</f>
         <v>3.8</v>
       </c>
-      <c r="N13" s="22" t="str">
+      <c r="O13" s="22" t="str">
         <f>VLOOKUP(D13,[1]!VolumeType[#All],2,FALSE)</f>
         <v>Artifact</v>
       </c>
-      <c r="O13" s="23" t="str">
+      <c r="P13" s="23" t="str">
         <f>VLOOKUP(D13,[1]!VolumeType[#All],3,FALSE)</f>
         <v>None</v>
       </c>
-      <c r="P13" s="24" t="str">
-        <f>VLOOKUP(D13,[1]!Colors[#All],3,FALSE)</f>
-        <v>z Wire</v>
-      </c>
-      <c r="Q13" s="25" t="str">
+      <c r="Q13" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D13,[1]!Colors[#All],3,FALSE))</f>
+        <v>Transluce - Lila</v>
+      </c>
+      <c r="R13" s="25" t="str">
         <f>IFERROR(VLOOKUP(D13,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R13" s="26" t="str">
+      <c r="S13" s="26" t="str">
         <f>IFERROR(VLOOKUP(D13,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S13" s="27" t="str">
+      <c r="T13" s="27" t="str">
         <f>IFERROR(VLOOKUP(D13,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T13" s="25">
+      <c r="U13" s="25">
         <f>IFERROR(VLOOKUP(D13,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v>1800</v>
       </c>
-      <c r="U13" s="27">
+      <c r="V13" s="27">
         <f>IFERROR(VLOOKUP(D13,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v>29768</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="36"/>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="35"/>
-      <c r="J14" s="19" t="str">
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="K14" s="19" t="str">
         <f>VLOOKUP(D14,[1]!Dictionary[#All],3,FALSE)</f>
         <v>Skin</v>
       </c>
-      <c r="K14" s="20">
+      <c r="L14" s="20">
         <f>VLOOKUP(D14,[1]!Dictionary[#All],4,FALSE)</f>
         <v>7163</v>
       </c>
-      <c r="L14" s="20" t="str">
+      <c r="M14" s="20" t="str">
         <f>VLOOKUP(D14,[1]!Dictionary[#All],5,FALSE)</f>
         <v>FMA</v>
       </c>
-      <c r="M14" s="21" t="str">
+      <c r="N14" s="21" t="str">
         <f>VLOOKUP(D14,[1]!Dictionary[#All],6,FALSE)</f>
         <v>3.2</v>
       </c>
-      <c r="N14" s="22" t="str">
+      <c r="O14" s="22" t="str">
         <f>VLOOKUP(D14,[1]!VolumeType[#All],2,FALSE)</f>
         <v>Organ</v>
       </c>
-      <c r="O14" s="23" t="str">
+      <c r="P14" s="23" t="str">
         <f>VLOOKUP(D14,[1]!VolumeType[#All],3,FALSE)</f>
         <v>Organ</v>
       </c>
-      <c r="P14" s="24" t="str">
-        <f>VLOOKUP(D14,[1]!Colors[#All],3,FALSE)</f>
+      <c r="Q14" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D14,[1]!Colors[#All],3,FALSE))</f>
         <v>z Skin</v>
       </c>
-      <c r="Q14" s="25" t="str">
+      <c r="R14" s="25" t="str">
         <f>IFERROR(VLOOKUP(D14,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R14" s="26" t="str">
+      <c r="S14" s="26" t="str">
         <f>IFERROR(VLOOKUP(D14,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S14" s="27" t="str">
+      <c r="T14" s="27" t="str">
         <f>IFERROR(VLOOKUP(D14,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T14" s="25" t="str">
+      <c r="U14" s="25" t="str">
         <f>IFERROR(VLOOKUP(D14,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U14" s="27" t="str">
+      <c r="V14" s="27" t="str">
         <f>IFERROR(VLOOKUP(D14,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D15" s="31" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D15" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="15"/>
-      <c r="J15" s="19" t="str">
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="K15" s="19" t="str">
         <f>VLOOKUP(D15,[1]!Dictionary[#All],3,FALSE)</f>
         <v>Artifact</v>
       </c>
-      <c r="K15" s="20">
+      <c r="L15" s="20">
         <f>VLOOKUP(D15,[1]!Dictionary[#All],4,FALSE)</f>
         <v>11296</v>
       </c>
-      <c r="L15" s="20" t="str">
+      <c r="M15" s="20" t="str">
         <f>VLOOKUP(D15,[1]!Dictionary[#All],5,FALSE)</f>
         <v>RADLEX</v>
       </c>
-      <c r="M15" s="21">
+      <c r="N15" s="21">
         <f>VLOOKUP(D15,[1]!Dictionary[#All],6,FALSE)</f>
         <v>3.8</v>
       </c>
-      <c r="N15" s="22" t="str">
+      <c r="O15" s="22" t="str">
         <f>VLOOKUP(D15,[1]!VolumeType[#All],2,FALSE)</f>
         <v>Artifact</v>
       </c>
-      <c r="O15" s="23" t="str">
+      <c r="P15" s="23" t="str">
         <f>VLOOKUP(D15,[1]!VolumeType[#All],3,FALSE)</f>
         <v>None</v>
       </c>
-      <c r="P15" s="24" t="str">
-        <f>VLOOKUP(D15,[1]!Colors[#All],3,FALSE)</f>
+      <c r="Q15" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D15,[1]!Colors[#All],3,FALSE))</f>
         <v>z RO Helper</v>
       </c>
-      <c r="Q15" s="25" t="str">
+      <c r="R15" s="25" t="str">
         <f>IFERROR(VLOOKUP(D15,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R15" s="26" t="str">
+      <c r="S15" s="26" t="str">
         <f>IFERROR(VLOOKUP(D15,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S15" s="27" t="str">
+      <c r="T15" s="27" t="str">
         <f>IFERROR(VLOOKUP(D15,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T15" s="25" t="str">
+      <c r="U15" s="25" t="str">
         <f>IFERROR(VLOOKUP(D15,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U15" s="27" t="str">
+      <c r="V15" s="27" t="str">
         <f>IFERROR(VLOOKUP(D15,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D16" s="31" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D16" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="E16" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="15"/>
-      <c r="J16" s="19" t="str">
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="K16" s="19" t="str">
         <f>VLOOKUP(D16,[1]!Dictionary[#All],3,FALSE)</f>
         <v>Artifact</v>
       </c>
-      <c r="K16" s="20">
+      <c r="L16" s="20">
         <f>VLOOKUP(D16,[1]!Dictionary[#All],4,FALSE)</f>
         <v>11296</v>
       </c>
-      <c r="L16" s="20" t="str">
+      <c r="M16" s="20" t="str">
         <f>VLOOKUP(D16,[1]!Dictionary[#All],5,FALSE)</f>
         <v>RADLEX</v>
       </c>
-      <c r="M16" s="21">
+      <c r="N16" s="21">
         <f>VLOOKUP(D16,[1]!Dictionary[#All],6,FALSE)</f>
         <v>3.8</v>
       </c>
-      <c r="N16" s="22" t="str">
+      <c r="O16" s="22" t="str">
         <f>VLOOKUP(D16,[1]!VolumeType[#All],2,FALSE)</f>
         <v>Artifact</v>
       </c>
-      <c r="O16" s="23" t="str">
+      <c r="P16" s="23" t="str">
         <f>VLOOKUP(D16,[1]!VolumeType[#All],3,FALSE)</f>
         <v>None</v>
       </c>
-      <c r="P16" s="24" t="str">
-        <f>VLOOKUP(D16,[1]!Colors[#All],3,FALSE)</f>
+      <c r="Q16" s="24" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D16,[1]!Colors[#All],3,FALSE))</f>
         <v>z RO Helper</v>
       </c>
-      <c r="Q16" s="25" t="str">
+      <c r="R16" s="25" t="str">
         <f>IFERROR(VLOOKUP(D16,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R16" s="26" t="str">
+      <c r="S16" s="26" t="str">
         <f>IFERROR(VLOOKUP(D16,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S16" s="27" t="str">
+      <c r="T16" s="27" t="str">
         <f>IFERROR(VLOOKUP(D16,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T16" s="25" t="str">
+      <c r="U16" s="25" t="str">
         <f>IFERROR(VLOOKUP(D16,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U16" s="27" t="str">
+      <c r="V16" s="27" t="str">
         <f>IFERROR(VLOOKUP(D16,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="31" t="s">
+    <row r="17" spans="4:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-      <c r="J17" s="37" t="str">
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="K17" s="37" t="str">
         <f>VLOOKUP(D17,[1]!Dictionary[#All],3,FALSE)</f>
         <v>Artifact</v>
       </c>
-      <c r="K17" s="38">
+      <c r="L17" s="38">
         <f>VLOOKUP(D17,[1]!Dictionary[#All],4,FALSE)</f>
         <v>11296</v>
       </c>
-      <c r="L17" s="38" t="str">
+      <c r="M17" s="38" t="str">
         <f>VLOOKUP(D17,[1]!Dictionary[#All],5,FALSE)</f>
         <v>RADLEX</v>
       </c>
-      <c r="M17" s="39">
+      <c r="N17" s="39">
         <f>VLOOKUP(D17,[1]!Dictionary[#All],6,FALSE)</f>
         <v>3.8</v>
       </c>
-      <c r="N17" s="40" t="str">
+      <c r="O17" s="40" t="str">
         <f>VLOOKUP(D17,[1]!VolumeType[#All],2,FALSE)</f>
         <v>Artifact</v>
       </c>
-      <c r="O17" s="41" t="str">
+      <c r="P17" s="41" t="str">
         <f>VLOOKUP(D17,[1]!VolumeType[#All],3,FALSE)</f>
         <v>None</v>
       </c>
-      <c r="P17" s="42" t="str">
-        <f>VLOOKUP(D17,[1]!Colors[#All],3,FALSE)</f>
+      <c r="Q17" s="42" t="str">
+        <f>IF(Table5337911[[#This Row],[ColorAndStyle]]&lt;&gt;0,Table5337911[[#This Row],[ColorAndStyle]],VLOOKUP(D17,[1]!Colors[#All],3,FALSE))</f>
         <v>z RO Helper</v>
       </c>
-      <c r="Q17" s="43" t="str">
+      <c r="R17" s="43" t="str">
         <f>IFERROR(VLOOKUP(D17,[1]!DVH_lines[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R17" s="44" t="str">
+      <c r="S17" s="44" t="str">
         <f>IFERROR(VLOOKUP(D17,[1]!DVH_lines[#Data],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="S17" s="45" t="str">
+      <c r="T17" s="45" t="str">
         <f>IFERROR(VLOOKUP(D17,[1]!DVH_lines[#Data],4,FALSE),"")</f>
         <v/>
       </c>
-      <c r="T17" s="43" t="str">
+      <c r="U17" s="43" t="str">
         <f>IFERROR(VLOOKUP(D17,[1]!SearchCT[#Data],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="U17" s="45" t="str">
+      <c r="V17" s="45" t="str">
         <f>IFERROR(VLOOKUP(D17,[1]!SearchCT[#Data],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="U1:V1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:H1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="R1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="93" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3100,40 +3032,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="51"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="J1" s="48" t="s">
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="J1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="48" t="s">
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="51"/>
+      <c r="O1" s="52"/>
       <c r="P1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="48" t="s">
+      <c r="R1" s="52"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="49"/>
+      <c r="U1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3927,40 +3859,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="50"/>
+      <c r="B1" s="51"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="J1" s="48" t="s">
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="J1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="48" t="s">
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="51"/>
+      <c r="O1" s="52"/>
       <c r="P1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="48" t="s">
+      <c r="R1" s="52"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="49"/>
+      <c r="U1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">

</xml_diff>